<commit_message>
Methods implemented: groups.getBanned groups.getById groups.getMembers groups.isMember messages.createChat messages.delete
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java_labs\java-vk-bots-long-poll-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88427FA3-2B42-4774-A354-52EED689CE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -19,10 +20,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Methods!$A$1:$C$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Statistics!$A$1:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -625,7 +635,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -817,7 +827,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -843,7 +852,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-UA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1008,7 +1017,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="ru-UA"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1033,9 +1042,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1071,10 +1078,10 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1147,7 +1154,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-UA"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1193,7 +1200,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-UA"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1862,7 +1869,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2142,11 +2155,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,8 +2429,8 @@
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>25</v>
+      <c r="C23" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2427,8 +2440,8 @@
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>25</v>
+      <c r="C24" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,8 +2506,8 @@
       <c r="B30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>25</v>
+      <c r="C30" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2526,8 +2539,8 @@
       <c r="B33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>25</v>
+      <c r="C33" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2603,8 +2616,8 @@
       <c r="B40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>25</v>
+      <c r="C40" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2614,8 +2627,8 @@
       <c r="B41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>25</v>
+      <c r="C41" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3213,16 +3226,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C95"/>
+  <autoFilter ref="A1:C95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
@@ -3264,7 +3277,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3273,7 +3286,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Methods implemented: messages.deleteChatPhoto messages.deleteConversation messages.edit messages.getByConversationMessageId messages.editChat messages.getById messages.getConversationMembers messages.getConversations
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88427FA3-2B42-4774-A354-52EED689CE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37E349D-A4E3-4442-B1AD-937EF13418B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="198">
   <si>
     <t>appWidgets.getAppImages</t>
   </si>
@@ -630,6 +630,9 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1081,10 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2158,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,7 +2535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>65</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>67</v>
       </c>
@@ -2554,7 +2557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>69</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>78</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
@@ -2609,7 +2612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>82</v>
       </c>
@@ -2620,7 +2623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>84</v>
       </c>
@@ -2631,81 +2634,84 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>25</v>
+      <c r="C48" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2715,8 +2721,8 @@
       <c r="B49" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>25</v>
+      <c r="C49" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3277,7 +3283,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3286,7 +3292,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Methods implemented: groups.getConversationsById groups.getHistory groups.getHistoryAttachments groups.getInviteLink messages.pin messages.restore messages.removeChatUser messages.searchConversations
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37E349D-A4E3-4442-B1AD-937EF13418B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC23D5-725C-4938-940B-C6CAFD491D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="198">
   <si>
     <t>appWidgets.getAppImages</t>
   </si>
@@ -1075,16 +1075,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2162,7 +2162,7 @@
   <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,7 +2714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>99</v>
       </c>
@@ -2725,40 +2725,46 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -2769,18 +2775,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>112</v>
       </c>
@@ -2802,7 +2808,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>114</v>
       </c>
@@ -2813,7 +2819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>116</v>
       </c>
@@ -2824,7 +2830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>117</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>118</v>
       </c>
@@ -2846,40 +2852,40 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C61" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C61" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>125</v>
       </c>
@@ -2897,8 +2903,8 @@
       <c r="B65" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="15" t="s">
-        <v>25</v>
+      <c r="C65" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3265,7 +3271,7 @@
       </c>
       <c r="B2">
         <f>COUNTIFS(Methods!$C:$C,A2)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,7 +3289,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3292,7 +3298,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Methods implemented: messages.markAsAnsweredConversation messages.markAsImportantConversation messages.markAsRead photos.getOwnerCoverPhotoUploadServer photos.saveOwnerCoverPhoto wall.closeComments wall.openComments wall.createComment users.get
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC23D5-725C-4938-940B-C6CAFD491D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D08CC00-CB6F-4948-86B3-30BC805D117E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1075,16 +1075,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2161,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,8 +2826,8 @@
       <c r="B58" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>24</v>
+      <c r="C58" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2837,8 +2837,8 @@
       <c r="B59" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>24</v>
+      <c r="C59" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2848,8 +2848,8 @@
       <c r="B60" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="17" t="s">
-        <v>24</v>
+      <c r="C60" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2936,8 +2936,8 @@
       <c r="B68" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C68" s="15" t="s">
-        <v>25</v>
+      <c r="C68" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2958,8 +2958,8 @@
       <c r="B70" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="15" t="s">
-        <v>25</v>
+      <c r="C70" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2980,8 +2980,8 @@
       <c r="B72" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="15" t="s">
-        <v>25</v>
+      <c r="C72" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3145,8 +3145,8 @@
       <c r="B87" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C87" s="15" t="s">
-        <v>25</v>
+      <c r="C87" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,8 +3156,8 @@
       <c r="B88" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="17" t="s">
-        <v>24</v>
+      <c r="C88" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3167,8 +3167,8 @@
       <c r="B89" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="17" t="s">
-        <v>24</v>
+      <c r="C89" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,8 +3178,8 @@
       <c r="B90" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="17" t="s">
-        <v>24</v>
+      <c r="C90" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
       <c r="B91" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="17" t="s">
-        <v>24</v>
+      <c r="C91" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3200,8 +3200,8 @@
       <c r="B92" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C92" s="17" t="s">
-        <v>24</v>
+      <c r="C92" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3211,8 +3211,8 @@
       <c r="B93" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C93" s="17" t="s">
-        <v>24</v>
+      <c r="C93" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3222,8 +3222,8 @@
       <c r="B94" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C94" s="17" t="s">
-        <v>24</v>
+      <c r="C94" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3233,8 +3233,8 @@
       <c r="B95" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C95" s="17" t="s">
-        <v>24</v>
+      <c r="C95" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3248,7 +3248,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="B2">
         <f>COUNTIFS(Methods!$C:$C,A2)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="B3">
         <f>COUNTIFS(Methods!$C:$C,A3)</f>
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
API methods are implemented. Refactored VkApi class.
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D08CC00-CB6F-4948-86B3-30BC805D117E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ECC36B-D19D-4EDD-895C-42D320A1446C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -754,13 +754,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -1075,16 +1068,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2159,10 +2152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2181,7 @@
       </c>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2199,7 +2193,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2211,7 +2205,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2223,7 +2217,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2229,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2241,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2326,7 +2320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
@@ -2377,8 +2371,8 @@
       <c r="B18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>24</v>
+      <c r="C18" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,8 +2382,8 @@
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>24</v>
+      <c r="C19" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,8 +2393,8 @@
       <c r="B20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>24</v>
+      <c r="C20" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,8 +2404,8 @@
       <c r="B21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>24</v>
+      <c r="C21" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,8 +2415,8 @@
       <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>24</v>
+      <c r="C22" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2454,8 +2448,8 @@
       <c r="B25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>24</v>
+      <c r="C25" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,8 +2459,8 @@
       <c r="B26" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>24</v>
+      <c r="C26" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,8 +2470,8 @@
       <c r="B27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>24</v>
+      <c r="C27" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2498,8 +2492,8 @@
       <c r="B29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>24</v>
+      <c r="C29" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2520,8 +2514,8 @@
       <c r="B31" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>24</v>
+      <c r="C31" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2531,8 +2525,8 @@
       <c r="B32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>24</v>
+      <c r="C32" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,8 +2547,8 @@
       <c r="B34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>24</v>
+      <c r="C34" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,8 +2558,8 @@
       <c r="B35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>24</v>
+      <c r="C35" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2575,19 +2569,19 @@
       <c r="B36" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>24</v>
+      <c r="C37" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2597,19 +2591,19 @@
       <c r="B38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>24</v>
+      <c r="C39" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2764,7 +2758,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -2786,7 +2780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
@@ -2797,18 +2791,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C56" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>114</v>
       </c>
@@ -2885,7 +2879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>125</v>
       </c>
@@ -2918,7 +2912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>131</v>
       </c>
@@ -2929,7 +2923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>133</v>
       </c>
@@ -2984,7 +2978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>148</v>
       </c>
@@ -2995,7 +2989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>150</v>
       </c>
@@ -3006,7 +3000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>152</v>
       </c>
@@ -3017,125 +3011,125 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>154</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C77" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>158</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C79" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C81" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C82" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C83" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C84" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>172</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>174</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C86" s="17" t="s">
-        <v>24</v>
+      <c r="C86" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3156,8 +3150,8 @@
       <c r="B88" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="15" t="s">
-        <v>25</v>
+      <c r="C88" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3167,8 +3161,8 @@
       <c r="B89" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="15" t="s">
-        <v>25</v>
+      <c r="C89" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3178,8 +3172,8 @@
       <c r="B90" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="15" t="s">
-        <v>25</v>
+      <c r="C90" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3189,8 +3183,8 @@
       <c r="B91" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="15" t="s">
-        <v>25</v>
+      <c r="C91" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3200,8 +3194,8 @@
       <c r="B92" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C92" s="15" t="s">
-        <v>25</v>
+      <c r="C92" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3238,8 +3232,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C95" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Implemeted"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3247,8 +3248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,25 +3272,25 @@
       </c>
       <c r="B2">
         <f>COUNTIFS(Methods!$C:$C,A2)</f>
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B3">
         <f>COUNTIFS(Methods!$C:$C,A3)</f>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3298,7 +3299,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented methods: stories.delete, stories.get, stories.getById, stories.getPhotoUploadServer, stories.getReplies, stories.getStats
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ECC36B-D19D-4EDD-895C-42D320A1446C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C50FC-2895-4EDB-AC78-D788243C7A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Methods!$A$1:$C$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Methods!$A$1:$C$96</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Statistics!$A$1:$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="200">
   <si>
     <t>appWidgets.getAppImages</t>
   </si>
@@ -633,13 +633,19 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>messages.sendMessageEventAnswer</t>
+  </si>
+  <si>
+    <t>Dispatches an event with an action that will occur when the callback button is clicked.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +666,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -716,7 +730,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -761,6 +775,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1068,16 +1085,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,11 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A95"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,7 +2197,7 @@
       </c>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2193,7 +2209,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2205,7 +2221,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2233,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2229,7 +2245,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -2241,7 +2257,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2320,7 +2336,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
@@ -2573,7 +2589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -2595,7 +2611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
@@ -2758,7 +2774,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -2780,7 +2796,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
@@ -2791,7 +2807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>112</v>
       </c>
@@ -2802,7 +2818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>114</v>
       </c>
@@ -2879,7 +2895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>125</v>
       </c>
@@ -2912,23 +2928,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B68" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>14</v>
@@ -2936,219 +2952,219 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>19</v>
+        <v>134</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="C71" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="C72" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B73" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="C73" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C77" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="C78" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="C79" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C79" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="C80" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="C81" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C81" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="C82" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B83" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C82" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+      <c r="C83" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B84" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C83" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="C84" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B85" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C84" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="C85" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B86" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>14</v>
+      <c r="C86" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>19</v>
+        <v>175</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>19</v>
@@ -3156,10 +3172,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>19</v>
@@ -3167,10 +3183,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>19</v>
@@ -3178,32 +3194,32 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B92" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+      <c r="C92" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B93" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>19</v>
@@ -3211,10 +3227,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>19</v>
@@ -3222,23 +3238,28 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C96" s="14" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C95" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Implemeted"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3248,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,7 +3293,7 @@
       </c>
       <c r="B2">
         <f>COUNTIFS(Methods!$C:$C,A2)</f>
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,7 +3311,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3299,7 +3320,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3308,7 +3329,7 @@
       </c>
       <c r="B6" s="6">
         <f>SUM(B2:B5)</f>
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented methods: stories.getVideoUploadServer, stories.getViewers
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C50FC-2895-4EDB-AC78-D788243C7A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612AB1-AD65-4608-B009-85B34D4D1638}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,10 +1091,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2172,7 +2172,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,8 +3111,8 @@
       <c r="B83" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="15" t="s">
-        <v>25</v>
+      <c r="C83" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added methods: stories.hideAllReplies, stories.hideReply, stories.save Added events support: message_allow, message_deny
</commit_message>
<xml_diff>
--- a/Methods_implementation.xlsx
+++ b/Methods_implementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen\IdeaProjects\java-vk-bots-long-poll-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8181EC-763F-482F-B8D8-76D7A66DFECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9A6916-8BBB-4AF9-9D49-8DA3670EAFF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,10 +1091,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2172,7 +2172,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3133,8 +3133,8 @@
       <c r="B85" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="15" t="s">
-        <v>25</v>
+      <c r="C85" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,8 +3144,8 @@
       <c r="B86" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="15" t="s">
-        <v>25</v>
+      <c r="C86" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3155,8 +3155,8 @@
       <c r="B87" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="15" t="s">
-        <v>25</v>
+      <c r="C87" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B4">
         <f>COUNTIFS(Methods!$C:$C,A4)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="B5">
         <f>COUNTIFS(Methods!$C:$C,A5)</f>
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>